<commit_message>
Correctif généraux et script BD v2
</commit_message>
<xml_diff>
--- a/Base de données/Excel/Programme.xlsx
+++ b/Base de données/Excel/Programme.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GauCa1532715.CEGEPJONQUIERE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!ProjetFinal\Base de données\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
-    <t>commentaire</t>
-  </si>
-  <si>
     <t>Soins infirmiers</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>codeProgramme</t>
+  </si>
+  <si>
+    <t>nom</t>
   </si>
 </sst>
 </file>
@@ -410,17 +410,17 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -428,7 +428,7 @@
         <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
         <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,7 +444,7 @@
         <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -452,7 +452,7 @@
         <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -460,7 +460,7 @@
         <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -468,7 +468,7 @@
         <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -476,7 +476,7 @@
         <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -484,7 +484,7 @@
         <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -492,7 +492,7 @@
         <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -500,7 +500,7 @@
         <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -508,7 +508,7 @@
         <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -516,7 +516,7 @@
         <v>351</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -524,7 +524,7 @@
         <v>388</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>410</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -540,7 +540,7 @@
         <v>412</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>420</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -556,7 +556,7 @@
         <v>500</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>510</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
         <v>582</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -580,7 +580,7 @@
         <v>589</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>700</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge master into Fabrice
</commit_message>
<xml_diff>
--- a/Base de données/Excel/Programme.xlsx
+++ b/Base de données/Excel/Programme.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GauCa1532715.CEGEPJONQUIERE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!ProjetFinal\Base de données\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
-    <t>commentaire</t>
-  </si>
-  <si>
     <t>Soins infirmiers</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>codeProgramme</t>
+  </si>
+  <si>
+    <t>nom</t>
   </si>
 </sst>
 </file>
@@ -410,17 +410,17 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -428,7 +428,7 @@
         <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
         <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,7 +444,7 @@
         <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -452,7 +452,7 @@
         <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -460,7 +460,7 @@
         <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -468,7 +468,7 @@
         <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -476,7 +476,7 @@
         <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -484,7 +484,7 @@
         <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -492,7 +492,7 @@
         <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -500,7 +500,7 @@
         <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -508,7 +508,7 @@
         <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -516,7 +516,7 @@
         <v>351</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -524,7 +524,7 @@
         <v>388</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>410</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -540,7 +540,7 @@
         <v>412</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>420</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -556,7 +556,7 @@
         <v>500</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>510</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
         <v>582</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -580,7 +580,7 @@
         <v>589</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>700</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
envoie vers branche distante
</commit_message>
<xml_diff>
--- a/Base de données/Excel/Programme.xlsx
+++ b/Base de données/Excel/Programme.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GauCa1532715.CEGEPJONQUIERE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!ProjetFinal\Base de données\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
-    <t>commentaire</t>
-  </si>
-  <si>
     <t>Soins infirmiers</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>codeProgramme</t>
+  </si>
+  <si>
+    <t>nom</t>
   </si>
 </sst>
 </file>
@@ -410,17 +410,17 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -428,7 +428,7 @@
         <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
         <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,7 +444,7 @@
         <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -452,7 +452,7 @@
         <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -460,7 +460,7 @@
         <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -468,7 +468,7 @@
         <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -476,7 +476,7 @@
         <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -484,7 +484,7 @@
         <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -492,7 +492,7 @@
         <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -500,7 +500,7 @@
         <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -508,7 +508,7 @@
         <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -516,7 +516,7 @@
         <v>351</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -524,7 +524,7 @@
         <v>388</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>410</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -540,7 +540,7 @@
         <v>412</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>420</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -556,7 +556,7 @@
         <v>500</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>510</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
         <v>582</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -580,7 +580,7 @@
         <v>589</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>700</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>